<commit_message>
Modelatge Països, continents, subcontinents
</commit_message>
<xml_diff>
--- a/content/drafts/entitats/Codis_Territori_Continents.xlsx
+++ b/content/drafts/entitats/Codis_Territori_Continents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\layatsal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAA\CTTI\02.Projecte_DadesRef\_____c6\01.CATaleg\07.Proposta_noves_ER\04.Cataleg_Entitats_Modelades.v03\07.Continents_paisos\Propostes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551AEDF8-EFAA-4A3D-ABAE-F9AF5874690A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667E9EB7-C570-454F-96EE-F58DB9F665AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-1668" windowWidth="23256" windowHeight="13176" xr2:uid="{9AAF9F5B-2A3E-4EB7-9E37-F6CB3D83CC8F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{9AAF9F5B-2A3E-4EB7-9E37-F6CB3D83CC8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Continents" sheetId="1" r:id="rId1"/>
@@ -36,42 +36,18 @@
     <t>Nom Taula:</t>
   </si>
   <si>
-    <t>Identificador</t>
-  </si>
-  <si>
-    <t>Nom Català</t>
-  </si>
-  <si>
-    <t>00001</t>
-  </si>
-  <si>
     <t>Àfrica</t>
   </si>
   <si>
-    <t>00002</t>
-  </si>
-  <si>
     <t>Amèrica</t>
   </si>
   <si>
-    <t>00003</t>
-  </si>
-  <si>
     <t>Antàrtida i Territoris Propers</t>
   </si>
   <si>
-    <t>00004</t>
-  </si>
-  <si>
     <t>Àsia</t>
   </si>
   <si>
-    <t>00005</t>
-  </si>
-  <si>
-    <t>00006</t>
-  </si>
-  <si>
     <t>Europa</t>
   </si>
   <si>
@@ -81,16 +57,40 @@
     <t>No consta</t>
   </si>
   <si>
-    <t>99998</t>
-  </si>
-  <si>
     <t>Codis_Continents</t>
   </si>
   <si>
-    <t>99999</t>
-  </si>
-  <si>
-    <t>Altres/diversos</t>
+    <t>Codi</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>Altres/Diversos</t>
   </si>
 </sst>
 </file>
@@ -214,8 +214,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF418719-6AC3-41A5-8113-41D87D46EF02}" name="Table1" displayName="Table1" ref="A3:B11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9A1D12C3-B5BA-4983-9E6C-9D229CD51903}" name="Identificador" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{D539960F-07C7-41C0-B015-C8071841C528}" name="Nom Català" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9A1D12C3-B5BA-4983-9E6C-9D229CD51903}" name="Codi" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{D539960F-07C7-41C0-B015-C8071841C528}" name="Nom" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -522,86 +522,86 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="27.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -615,7 +615,7 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A4:B11" numberStoredAsText="1"/>
+    <ignoredError sqref="B4 B5 B6 B7 B8 B9 B10" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>